<commit_message>
newer design, added cert, small changes
</commit_message>
<xml_diff>
--- a/public/data/portfolio/portfolio.xlsx
+++ b/public/data/portfolio/portfolio.xlsx
@@ -609,12 +609,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Finally completed chess game to play locally. Try this out here: https://jasurgraduate.github.io/chess/</t>
+          <t>Finally completed chess game to play locally. Try this out here: https://uzChess.vercel.app</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://blogger.googleusercontent.com/img/a/AVvXsEjtKFjW2CB7bQ7Jd5s_LqGg1g1upuVBLXxozwN5ECHbFCS6bdmOmuql8RSTcrldQP_FLOVgJ1MnwEtdxyyk8w9QzeXAg-SV25p2QED3Yg4-YUCjSVdYSkvhufOQ8fIELlbxp8bbo-itc96u9tDN5dwazwcEMNC5JlpSrc-86p7owJP_oJ9D3P0P4Xf92Gg</t>
+          <t>https://blogger.googleusercontent.com/img/a/AVvXsEhBKl54c5hfCPv11-NQ9vAH6bt5CYqbTBKmIWCypW_2evRKtDGLNksCEGVYtvBoqCUK4oUMQHo0PKd89jOawDj5A7RE55HKjhbDXgm_UqQjHi8pDTHRc6NpIV6-UfrQRuT8Z4apXFa2rwipiAauVzuWzoXqurpBGmJwh4eN8pPLvmTcUem_9Bo6A0Ncdlo</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
portfolio fix, some cleanups
</commit_message>
<xml_diff>
--- a/public/data/portfolio/portfolio.xlsx
+++ b/public/data/portfolio/portfolio.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,7 +631,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>I created a quiz of testing your Hangul knowledge. And in the end according to your result you can get a personal certificate like this. Give it a try! You will love it! | https://jasurgraduate.github.io/Hangul/</t>
+          <t>I created a quiz of testing your Hangul knowledge. And in the end according to your result you can get a personal certificate like this. Give it a try! You will love it! | https://jasurlive.github.io/Hangul/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -680,7 +680,29 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://blogger.googleusercontent.com/img/b/R29vZ2xl/AVvXsEg5K2OMTFnxyqQZyad_adMoXysl85NsZnKH_-k0yIZFHWw9uvGlh7Ss-WpbM58XNw2NVMoytppUCjm7KD6ZFjtvtZ3CX2oEYwFEbXM07yYuOtxrSVoHVb6bvLXYBMTCsiHgDkpRrUF6wSvGOCDhMG6gV4uyumqzu1pltn8JrdgrsCCvs4nADX1Dvni62lg/s1919/Screenshot%202025-03-01%20174733.png</t>
+          <t>https://blogger.googleusercontent.com/img/a/AVvXsEhRneIHityZCfdxYN2EabHWzPEHpiqWFw9UFIPEzeBZNwjGyDQK-M4bQ2ZMCA8SdgZ_k1UYS-eKWhrU3uF_V87SKRyqE7Fi-TCW11UoEfGRvH-zfygoCGuV5hCOMyMA9Ty-Xzj9AjW5C7_B255wIj_ZSHP52H9ExRvatwOquMS-B99GUUv7_0x5k9TJ8p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-22 17:34:06</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>POS App for a local market in Daejeon</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Point Of Sale (POS) app for the local store. Inventory control, calculations of income and outcome. Works with any inventory. The excel sheet needs to be modified accordingly before using it.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://blogger.googleusercontent.com/img/b/R29vZ2xl/AVvXsEjA1FzCHoSKmitLjioCBqb4eMmq3MQAFdEnUhzNt5q6WthEYhnTavPmURhhQFcGI46EKgr9SokoE00hfF87GYdCmjUk3YZGgBMO6HW4V8t_tpgg2UHF0rZnVl8Df15AXWG7kZbBLCBQvlwbYBDHhZ3tPJDBGAWmwyVcI-UzfstOXxwSAb2UnIaet9xpYUQ/s1917/POS.png</t>
         </is>
       </c>
     </row>

</xml_diff>